<commit_message>
Updated implementation, added name to class mapping method.
</commit_message>
<xml_diff>
--- a/inst/extdata/class_map.xlsx
+++ b/inst/extdata/class_map.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="91">
   <si>
-    <t xml:space="preserve">Lipid.Maps.Main.Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LipidCategoryOrClass</t>
+    <t xml:space="preserve">LipidMapsCategoryOrClass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EposmolCategoryOrClass</t>
   </si>
   <si>
     <t xml:space="preserve">FA</t>
@@ -181,10 +181,10 @@
     <t xml:space="preserve">CL</t>
   </si>
   <si>
-    <t xml:space="preserve">#DLCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#LCL</t>
+    <t xml:space="preserve">DLCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCL</t>
   </si>
   <si>
     <t xml:space="preserve">PS-N</t>
@@ -307,6 +307,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -391,10 +392,10 @@
   <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.08"/>

</xml_diff>